<commit_message>
effect direction & min p_val
</commit_message>
<xml_diff>
--- a/beta_meta/output/meta_output.xlsx
+++ b/beta_meta/output/meta_output.xlsx
@@ -109,13 +109,13 @@
     <t>C</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>G</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>0.3711569546144358</v>
@@ -560,10 +560,10 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3">
-        <v>0.3653988847128944</v>
+        <v>-0.3653988847128944</v>
       </c>
       <c r="G3">
         <v>0.08871321095061897</v>
@@ -592,10 +592,10 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>0.3714916289836939</v>
@@ -627,10 +627,10 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
       <c r="F5">
         <v>0.5325639672023215</v>
@@ -665,7 +665,7 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>0.6437238974622098</v>
@@ -697,7 +697,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -735,10 +735,10 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8">
-        <v>-0.2593599748104452</v>
+        <v>0.2593599748104452</v>
       </c>
       <c r="G8">
         <v>0.1444105735983564</v>
@@ -767,13 +767,13 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9">
-        <v>0.3513041745623368</v>
+        <v>-0.3513041745623368</v>
       </c>
       <c r="G9">
         <v>0.03136179445042608</v>
@@ -802,10 +802,10 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>-0.292415627494133</v>
@@ -840,7 +840,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11">
         <v>0.3403853571739563</v>
@@ -872,10 +872,10 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>0.4527792954424879</v>
@@ -907,7 +907,7 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -942,7 +942,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>

</xml_diff>